<commit_message>
calculo do erro médio finalizado
</commit_message>
<xml_diff>
--- a/Análises/Erro_Medio.xlsx
+++ b/Análises/Erro_Medio.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,91 +449,451 @@
           <t>rfaz_complementar</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>rfax_Calibrated</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>rfay_Calibrated</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>rfaz_Calibrated</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>rfax_Calibrated_Complementar</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>rfay_Calibrated_Complementar</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>rfaz_Calibrated_Complementar</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>rfax_Kalman</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>rfay_Kalman</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>rfaz_Kalman</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>rfax_Kalman_Complementar</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>rfay_Kalman_Complementar</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>rfaz_Kalman_Complementar</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>rfax_LowPass</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>rfay_LowPass</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>rfaz_LowPass</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>rfax_LowPass_Complementar</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>rfay_LowPass_Complementar</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>rfaz_LowPass_Complementar</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_10_06_new.xlsx</t>
+          <t>HuGaDB_v2_various_11_10.xlsx</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14931.65134935305</v>
+        <v>14807.39958955224</v>
       </c>
       <c r="C2" t="n">
-        <v>10170.89648798521</v>
+        <v>7953.915858208956</v>
       </c>
       <c r="D2" t="n">
-        <v>11280.07987060998</v>
+        <v>15063.77197761194</v>
+      </c>
+      <c r="E2" t="n">
+        <v>14832.2690392696</v>
+      </c>
+      <c r="F2" t="n">
+        <v>8245.455821549089</v>
+      </c>
+      <c r="G2" t="n">
+        <v>14908.59204925946</v>
+      </c>
+      <c r="H2" t="n">
+        <v>14778.83729031424</v>
+      </c>
+      <c r="I2" t="n">
+        <v>8172.737508167273</v>
+      </c>
+      <c r="J2" t="n">
+        <v>14892.92057582166</v>
+      </c>
+      <c r="K2" t="n">
+        <v>14832.31953100904</v>
+      </c>
+      <c r="L2" t="n">
+        <v>8245.748897466483</v>
+      </c>
+      <c r="M2" t="n">
+        <v>14908.83361349311</v>
+      </c>
+      <c r="N2" t="n">
+        <v>14746.33048428659</v>
+      </c>
+      <c r="O2" t="n">
+        <v>8442.329954345214</v>
+      </c>
+      <c r="P2" t="n">
+        <v>14872.60883537152</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>14832.31271069421</v>
+      </c>
+      <c r="R2" t="n">
+        <v>8245.572445395423</v>
+      </c>
+      <c r="S2" t="n">
+        <v>14908.64410952065</v>
+      </c>
+      <c r="T2" t="n">
+        <v>14778.83816374273</v>
+      </c>
+      <c r="U2" t="n">
+        <v>8172.739845093281</v>
+      </c>
+      <c r="V2" t="n">
+        <v>14892.92159123434</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_11_11_new.xlsx</t>
+          <t>HuGaDB_v2_various_11_05.xlsx</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>11829.74033088235</v>
+        <v>13937.17502852486</v>
       </c>
       <c r="C3" t="n">
-        <v>9251.38194852941</v>
+        <v>8523.199771801143</v>
       </c>
       <c r="D3" t="n">
-        <v>16397.73290441177</v>
+        <v>17978.73496332518</v>
+      </c>
+      <c r="E3" t="n">
+        <v>14280.92830272896</v>
+      </c>
+      <c r="F3" t="n">
+        <v>7919.922032614335</v>
+      </c>
+      <c r="G3" t="n">
+        <v>18147.6504401353</v>
+      </c>
+      <c r="H3" t="n">
+        <v>14278.68993103921</v>
+      </c>
+      <c r="I3" t="n">
+        <v>8649.826574964518</v>
+      </c>
+      <c r="J3" t="n">
+        <v>18238.1961626419</v>
+      </c>
+      <c r="K3" t="n">
+        <v>14281.00854812641</v>
+      </c>
+      <c r="L3" t="n">
+        <v>7920.225878856423</v>
+      </c>
+      <c r="M3" t="n">
+        <v>18147.9363488878</v>
+      </c>
+      <c r="N3" t="n">
+        <v>14225.64936181829</v>
+      </c>
+      <c r="O3" t="n">
+        <v>8663.335574405006</v>
+      </c>
+      <c r="P3" t="n">
+        <v>18135.77537080874</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>14280.98356337628</v>
+      </c>
+      <c r="R3" t="n">
+        <v>7920.05425186803</v>
+      </c>
+      <c r="S3" t="n">
+        <v>18147.71761441338</v>
+      </c>
+      <c r="T3" t="n">
+        <v>14278.69099054619</v>
+      </c>
+      <c r="U3" t="n">
+        <v>8649.829148927131</v>
+      </c>
+      <c r="V3" t="n">
+        <v>18238.19756889311</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_11_10_new.xlsx</t>
+          <t>HuGaDB_v2_various_11_11.xlsx</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>14807.39958955224</v>
+        <v>11829.74033088235</v>
       </c>
       <c r="C4" t="n">
-        <v>7953.915858208956</v>
+        <v>9251.38194852941</v>
       </c>
       <c r="D4" t="n">
-        <v>15063.77197761194</v>
+        <v>16397.73290441177</v>
+      </c>
+      <c r="E4" t="n">
+        <v>12497.94065626246</v>
+      </c>
+      <c r="F4" t="n">
+        <v>7998.12435024294</v>
+      </c>
+      <c r="G4" t="n">
+        <v>16833.31828079451</v>
+      </c>
+      <c r="H4" t="n">
+        <v>12526.86884671705</v>
+      </c>
+      <c r="I4" t="n">
+        <v>9388.135371502229</v>
+      </c>
+      <c r="J4" t="n">
+        <v>16935.92996355598</v>
+      </c>
+      <c r="K4" t="n">
+        <v>12498.05210022044</v>
+      </c>
+      <c r="L4" t="n">
+        <v>7998.4056172529</v>
+      </c>
+      <c r="M4" t="n">
+        <v>16833.56269070167</v>
+      </c>
+      <c r="N4" t="n">
+        <v>12533.9579846165</v>
+      </c>
+      <c r="O4" t="n">
+        <v>9167.60182382823</v>
+      </c>
+      <c r="P4" t="n">
+        <v>16856.30258815029</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>12497.99466133898</v>
+      </c>
+      <c r="R4" t="n">
+        <v>7998.222016659432</v>
+      </c>
+      <c r="S4" t="n">
+        <v>16833.43726715629</v>
+      </c>
+      <c r="T4" t="n">
+        <v>12526.86979102234</v>
+      </c>
+      <c r="U4" t="n">
+        <v>9388.137211677464</v>
+      </c>
+      <c r="V4" t="n">
+        <v>16935.93234328322</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_10_08_new.xlsx</t>
+          <t>HuGaDB_v2_various_09_13.xlsx</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>14223.61604790419</v>
+        <v>17625.44300904977</v>
       </c>
       <c r="C5" t="n">
-        <v>9974.594251497007</v>
+        <v>8249.661063348416</v>
       </c>
       <c r="D5" t="n">
-        <v>11842.83473053892</v>
+        <v>14519.2603959276</v>
+      </c>
+      <c r="E5" t="n">
+        <v>18159.5803304528</v>
+      </c>
+      <c r="F5" t="n">
+        <v>7199.642955433131</v>
+      </c>
+      <c r="G5" t="n">
+        <v>14796.48949096544</v>
+      </c>
+      <c r="H5" t="n">
+        <v>18108.2490382552</v>
+      </c>
+      <c r="I5" t="n">
+        <v>8383.487541048511</v>
+      </c>
+      <c r="J5" t="n">
+        <v>14740.83766688324</v>
+      </c>
+      <c r="K5" t="n">
+        <v>18159.69112815594</v>
+      </c>
+      <c r="L5" t="n">
+        <v>7200.042028005981</v>
+      </c>
+      <c r="M5" t="n">
+        <v>14796.88386141371</v>
+      </c>
+      <c r="N5" t="n">
+        <v>18064.74218965656</v>
+      </c>
+      <c r="O5" t="n">
+        <v>8083.362944554536</v>
+      </c>
+      <c r="P5" t="n">
+        <v>14737.12921154324</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>18159.70816588891</v>
+      </c>
+      <c r="R5" t="n">
+        <v>7199.827205474953</v>
+      </c>
+      <c r="S5" t="n">
+        <v>14796.58783993799</v>
+      </c>
+      <c r="T5" t="n">
+        <v>18108.25152773898</v>
+      </c>
+      <c r="U5" t="n">
+        <v>8383.49084538534</v>
+      </c>
+      <c r="V5" t="n">
+        <v>14740.83976283365</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_10_09_new.xlsx</t>
+          <t>HuGaDB_v2_various_11_16.xlsx</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>14805.45829984544</v>
+        <v>12847.03674698795</v>
       </c>
       <c r="C6" t="n">
-        <v>11356.70955177743</v>
+        <v>6106.498915662651</v>
       </c>
       <c r="D6" t="n">
-        <v>12075.04955177743</v>
+        <v>14903.65192771084</v>
+      </c>
+      <c r="E6" t="n">
+        <v>12868.49658457479</v>
+      </c>
+      <c r="F6" t="n">
+        <v>6297.732737501094</v>
+      </c>
+      <c r="G6" t="n">
+        <v>14781.94872860021</v>
+      </c>
+      <c r="H6" t="n">
+        <v>12839.43053402774</v>
+      </c>
+      <c r="I6" t="n">
+        <v>6255.181407561256</v>
+      </c>
+      <c r="J6" t="n">
+        <v>14765.7281581002</v>
+      </c>
+      <c r="K6" t="n">
+        <v>12868.54362570449</v>
+      </c>
+      <c r="L6" t="n">
+        <v>6298.054155478666</v>
+      </c>
+      <c r="M6" t="n">
+        <v>14782.14875913802</v>
+      </c>
+      <c r="N6" t="n">
+        <v>12819.83091448499</v>
+      </c>
+      <c r="O6" t="n">
+        <v>6440.431357741434</v>
+      </c>
+      <c r="P6" t="n">
+        <v>14768.36047309495</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>12868.53874401658</v>
+      </c>
+      <c r="R6" t="n">
+        <v>6297.852728107064</v>
+      </c>
+      <c r="S6" t="n">
+        <v>14782.00525614004</v>
+      </c>
+      <c r="T6" t="n">
+        <v>12839.43131040384</v>
+      </c>
+      <c r="U6" t="n">
+        <v>6255.183737819907</v>
+      </c>
+      <c r="V6" t="n">
+        <v>14765.72933356888</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_10_05_new.xlsx</t>
+          <t>HuGaDB_v2_various_10_05.xlsx</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -545,309 +905,1389 @@
       <c r="D7" t="n">
         <v>13165.31831034483</v>
       </c>
+      <c r="E7" t="n">
+        <v>15319.86104468382</v>
+      </c>
+      <c r="F7" t="n">
+        <v>8164.671645904366</v>
+      </c>
+      <c r="G7" t="n">
+        <v>13589.16739035159</v>
+      </c>
+      <c r="H7" t="n">
+        <v>15394.6475704842</v>
+      </c>
+      <c r="I7" t="n">
+        <v>9097.61704713795</v>
+      </c>
+      <c r="J7" t="n">
+        <v>13529.18587392274</v>
+      </c>
+      <c r="K7" t="n">
+        <v>15320.06249136147</v>
+      </c>
+      <c r="L7" t="n">
+        <v>8165.053865692164</v>
+      </c>
+      <c r="M7" t="n">
+        <v>13589.54738624708</v>
+      </c>
+      <c r="N7" t="n">
+        <v>15407.83287532291</v>
+      </c>
+      <c r="O7" t="n">
+        <v>9003.445909163471</v>
+      </c>
+      <c r="P7" t="n">
+        <v>13526.88500284775</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>15319.9616863197</v>
+      </c>
+      <c r="R7" t="n">
+        <v>8164.792118098992</v>
+      </c>
+      <c r="S7" t="n">
+        <v>13589.21455092283</v>
+      </c>
+      <c r="T7" t="n">
+        <v>15394.64948979944</v>
+      </c>
+      <c r="U7" t="n">
+        <v>9097.619416505342</v>
+      </c>
+      <c r="V7" t="n">
+        <v>13529.1869797153</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_09_14_new.xlsx</t>
+          <t>HuGaDB_v2_various_10_07.xlsx</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17843.6866620306</v>
+        <v>13858.33795191451</v>
       </c>
       <c r="C8" t="n">
-        <v>8974.733685674548</v>
+        <v>7882.495173642031</v>
       </c>
       <c r="D8" t="n">
-        <v>14472.76744089012</v>
+        <v>13244.53943009795</v>
+      </c>
+      <c r="E8" t="n">
+        <v>14430.51816577734</v>
+      </c>
+      <c r="F8" t="n">
+        <v>7231.486005652007</v>
+      </c>
+      <c r="G8" t="n">
+        <v>13636.09277341717</v>
+      </c>
+      <c r="H8" t="n">
+        <v>14563.69017299241</v>
+      </c>
+      <c r="I8" t="n">
+        <v>8119.682973204003</v>
+      </c>
+      <c r="J8" t="n">
+        <v>13665.01592193292</v>
+      </c>
+      <c r="K8" t="n">
+        <v>14430.70056408834</v>
+      </c>
+      <c r="L8" t="n">
+        <v>7231.821017966325</v>
+      </c>
+      <c r="M8" t="n">
+        <v>13636.42975182154</v>
+      </c>
+      <c r="N8" t="n">
+        <v>14592.74466995821</v>
+      </c>
+      <c r="O8" t="n">
+        <v>8004.245271380375</v>
+      </c>
+      <c r="P8" t="n">
+        <v>13606.27779858292</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>14430.60104068352</v>
+      </c>
+      <c r="R8" t="n">
+        <v>7231.608354247678</v>
+      </c>
+      <c r="S8" t="n">
+        <v>13636.14329904148</v>
+      </c>
+      <c r="T8" t="n">
+        <v>14563.69170535713</v>
+      </c>
+      <c r="U8" t="n">
+        <v>8119.685399620617</v>
+      </c>
+      <c r="V8" t="n">
+        <v>13665.01699969221</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_10_10_new.xlsx</t>
+          <t>HuGaDB_v2_various_09_14.xlsx</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>14622.96586490939</v>
+        <v>17843.6866620306</v>
       </c>
       <c r="C9" t="n">
-        <v>7959.212883031301</v>
+        <v>8974.733685674548</v>
       </c>
       <c r="D9" t="n">
-        <v>13524.69584843493</v>
+        <v>14472.76744089012</v>
+      </c>
+      <c r="E9" t="n">
+        <v>18395.62635346909</v>
+      </c>
+      <c r="F9" t="n">
+        <v>7812.482362021551</v>
+      </c>
+      <c r="G9" t="n">
+        <v>14729.98504478367</v>
+      </c>
+      <c r="H9" t="n">
+        <v>18363.0782989524</v>
+      </c>
+      <c r="I9" t="n">
+        <v>9135.363047298983</v>
+      </c>
+      <c r="J9" t="n">
+        <v>14681.37112888108</v>
+      </c>
+      <c r="K9" t="n">
+        <v>18395.72408882782</v>
+      </c>
+      <c r="L9" t="n">
+        <v>7812.908466367601</v>
+      </c>
+      <c r="M9" t="n">
+        <v>14730.40566238175</v>
+      </c>
+      <c r="N9" t="n">
+        <v>18330.95679539273</v>
+      </c>
+      <c r="O9" t="n">
+        <v>8917.071998461826</v>
+      </c>
+      <c r="P9" t="n">
+        <v>14659.26720713725</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>18395.74256648702</v>
+      </c>
+      <c r="R9" t="n">
+        <v>7812.668481956678</v>
+      </c>
+      <c r="S9" t="n">
+        <v>14730.08556812428</v>
+      </c>
+      <c r="T9" t="n">
+        <v>18363.0805240388</v>
+      </c>
+      <c r="U9" t="n">
+        <v>9135.366401105202</v>
+      </c>
+      <c r="V9" t="n">
+        <v>14681.37322245553</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_11_13_new.xlsx</t>
+          <t>HuGaDB_v2_various_11_14.xlsx</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>11319.16363468635</v>
+        <v>13772.42130718954</v>
       </c>
       <c r="C10" t="n">
-        <v>9104.747859778598</v>
+        <v>7509.6677124183</v>
       </c>
       <c r="D10" t="n">
-        <v>17086.89215867158</v>
+        <v>15607.93477124183</v>
+      </c>
+      <c r="E10" t="n">
+        <v>13768.17866772594</v>
+      </c>
+      <c r="F10" t="n">
+        <v>7765.118419941776</v>
+      </c>
+      <c r="G10" t="n">
+        <v>15560.82183553135</v>
+      </c>
+      <c r="H10" t="n">
+        <v>13760.9754796769</v>
+      </c>
+      <c r="I10" t="n">
+        <v>7680.491600227538</v>
+      </c>
+      <c r="J10" t="n">
+        <v>15590.17995924278</v>
+      </c>
+      <c r="K10" t="n">
+        <v>13768.21068210141</v>
+      </c>
+      <c r="L10" t="n">
+        <v>7765.423876203129</v>
+      </c>
+      <c r="M10" t="n">
+        <v>15561.0908197746</v>
+      </c>
+      <c r="N10" t="n">
+        <v>13794.59975984022</v>
+      </c>
+      <c r="O10" t="n">
+        <v>7889.78215485358</v>
+      </c>
+      <c r="P10" t="n">
+        <v>15552.09897336157</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>13768.21593406423</v>
+      </c>
+      <c r="R10" t="n">
+        <v>7765.260558007146</v>
+      </c>
+      <c r="S10" t="n">
+        <v>15560.88415719828</v>
+      </c>
+      <c r="T10" t="n">
+        <v>13760.97603524893</v>
+      </c>
+      <c r="U10" t="n">
+        <v>7680.494463052324</v>
+      </c>
+      <c r="V10" t="n">
+        <v>15590.18146341005</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_11_07_new.xlsx</t>
+          <t>HuGaDB_v2_various_11_06.xlsx</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>14126.36040194884</v>
+        <v>13969.6899188876</v>
       </c>
       <c r="C11" t="n">
-        <v>8918.031035322778</v>
+        <v>8975.213982232523</v>
       </c>
       <c r="D11" t="n">
-        <v>18398.5653593179</v>
+        <v>18275.19065276168</v>
+      </c>
+      <c r="E11" t="n">
+        <v>14381.86718368347</v>
+      </c>
+      <c r="F11" t="n">
+        <v>8228.599770159153</v>
+      </c>
+      <c r="G11" t="n">
+        <v>18444.8884700614</v>
+      </c>
+      <c r="H11" t="n">
+        <v>14336.00388541924</v>
+      </c>
+      <c r="I11" t="n">
+        <v>9118.91713119371</v>
+      </c>
+      <c r="J11" t="n">
+        <v>18533.98175480851</v>
+      </c>
+      <c r="K11" t="n">
+        <v>14381.94355760898</v>
+      </c>
+      <c r="L11" t="n">
+        <v>8228.917715320687</v>
+      </c>
+      <c r="M11" t="n">
+        <v>18445.17972936039</v>
+      </c>
+      <c r="N11" t="n">
+        <v>14306.6201800411</v>
+      </c>
+      <c r="O11" t="n">
+        <v>9107.745638240423</v>
+      </c>
+      <c r="P11" t="n">
+        <v>18436.32512017371</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>14381.9360061231</v>
+      </c>
+      <c r="R11" t="n">
+        <v>8228.756900567565</v>
+      </c>
+      <c r="S11" t="n">
+        <v>18444.96988437049</v>
+      </c>
+      <c r="T11" t="n">
+        <v>14336.00508973927</v>
+      </c>
+      <c r="U11" t="n">
+        <v>9118.92020290839</v>
+      </c>
+      <c r="V11" t="n">
+        <v>18533.98332423488</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_10_07_new.xlsx</t>
+          <t>HuGaDB_v2_various_10_06.xlsx</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>13858.33795191451</v>
+        <v>14931.65134935305</v>
       </c>
       <c r="C12" t="n">
-        <v>7882.495173642031</v>
+        <v>10170.89648798521</v>
       </c>
       <c r="D12" t="n">
-        <v>13244.53943009795</v>
+        <v>11280.07987060998</v>
+      </c>
+      <c r="E12" t="n">
+        <v>15016.85285721521</v>
+      </c>
+      <c r="F12" t="n">
+        <v>10383.16896745793</v>
+      </c>
+      <c r="G12" t="n">
+        <v>11571.9213786454</v>
+      </c>
+      <c r="H12" t="n">
+        <v>14944.31767687549</v>
+      </c>
+      <c r="I12" t="n">
+        <v>10266.95613471346</v>
+      </c>
+      <c r="J12" t="n">
+        <v>11222.65503114695</v>
+      </c>
+      <c r="K12" t="n">
+        <v>15016.95219831958</v>
+      </c>
+      <c r="L12" t="n">
+        <v>10383.46503191809</v>
+      </c>
+      <c r="M12" t="n">
+        <v>11572.31313761855</v>
+      </c>
+      <c r="N12" t="n">
+        <v>15011.24862810759</v>
+      </c>
+      <c r="O12" t="n">
+        <v>10489.46281555647</v>
+      </c>
+      <c r="P12" t="n">
+        <v>11370.77186925589</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>15016.90137138346</v>
+      </c>
+      <c r="R12" t="n">
+        <v>10383.23718979097</v>
+      </c>
+      <c r="S12" t="n">
+        <v>11571.96554241858</v>
+      </c>
+      <c r="T12" t="n">
+        <v>14944.31866377234</v>
+      </c>
+      <c r="U12" t="n">
+        <v>10266.9574456336</v>
+      </c>
+      <c r="V12" t="n">
+        <v>11222.65588984168</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_09_16_new.xlsx</t>
+          <t>HuGaDB_v2_various_11_15.xlsx</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17312.43525076766</v>
+        <v>10976.76487804878</v>
       </c>
       <c r="C13" t="n">
-        <v>8609.975066530194</v>
+        <v>8074.643808630393</v>
       </c>
       <c r="D13" t="n">
-        <v>14215.28016376663</v>
+        <v>15927.9730956848</v>
+      </c>
+      <c r="E13" t="n">
+        <v>11632.45806666933</v>
+      </c>
+      <c r="F13" t="n">
+        <v>7071.167550278609</v>
+      </c>
+      <c r="G13" t="n">
+        <v>16401.28268965311</v>
+      </c>
+      <c r="H13" t="n">
+        <v>11620.90297435424</v>
+      </c>
+      <c r="I13" t="n">
+        <v>8226.222283493516</v>
+      </c>
+      <c r="J13" t="n">
+        <v>16437.16690035447</v>
+      </c>
+      <c r="K13" t="n">
+        <v>11632.6086556928</v>
+      </c>
+      <c r="L13" t="n">
+        <v>7071.501204912507</v>
+      </c>
+      <c r="M13" t="n">
+        <v>16401.51509344132</v>
+      </c>
+      <c r="N13" t="n">
+        <v>11619.08084301465</v>
+      </c>
+      <c r="O13" t="n">
+        <v>7974.796186696823</v>
+      </c>
+      <c r="P13" t="n">
+        <v>16409.32042790045</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>11632.53554465821</v>
+      </c>
+      <c r="R13" t="n">
+        <v>7071.283984074278</v>
+      </c>
+      <c r="S13" t="n">
+        <v>16401.3469617832</v>
+      </c>
+      <c r="T13" t="n">
+        <v>11620.90444527402</v>
+      </c>
+      <c r="U13" t="n">
+        <v>8226.224583099207</v>
+      </c>
+      <c r="V13" t="n">
+        <v>16437.16830726187</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_11_05_new.xlsx</t>
+          <t>HuGaDB_v2_various_10_08.xlsx</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>13937.17502852486</v>
+        <v>14223.61604790419</v>
       </c>
       <c r="C14" t="n">
-        <v>8523.199771801143</v>
+        <v>9974.594251497007</v>
       </c>
       <c r="D14" t="n">
-        <v>17978.73496332518</v>
+        <v>11842.83473053892</v>
+      </c>
+      <c r="E14" t="n">
+        <v>14265.71821301489</v>
+      </c>
+      <c r="F14" t="n">
+        <v>10067.98465731911</v>
+      </c>
+      <c r="G14" t="n">
+        <v>12175.36484982249</v>
+      </c>
+      <c r="H14" t="n">
+        <v>14215.7590284076</v>
+      </c>
+      <c r="I14" t="n">
+        <v>10000.86968108912</v>
+      </c>
+      <c r="J14" t="n">
+        <v>11816.88269599248</v>
+      </c>
+      <c r="K14" t="n">
+        <v>14265.81397441911</v>
+      </c>
+      <c r="L14" t="n">
+        <v>10068.24588039286</v>
+      </c>
+      <c r="M14" t="n">
+        <v>12175.7421037924</v>
+      </c>
+      <c r="N14" t="n">
+        <v>14216.19495216385</v>
+      </c>
+      <c r="O14" t="n">
+        <v>10168.12962082654</v>
+      </c>
+      <c r="P14" t="n">
+        <v>11968.92556124362</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>14265.77188818696</v>
+      </c>
+      <c r="R14" t="n">
+        <v>10068.07601820675</v>
+      </c>
+      <c r="S14" t="n">
+        <v>12175.40130563845</v>
+      </c>
+      <c r="T14" t="n">
+        <v>14215.76008713772</v>
+      </c>
+      <c r="U14" t="n">
+        <v>10000.87150076898</v>
+      </c>
+      <c r="V14" t="n">
+        <v>11816.88337656818</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_10_12_new.xlsx</t>
+          <t>HuGaDB_v2_various_11_04.xlsx</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>14675.19276887872</v>
+        <v>14340.75947834187</v>
       </c>
       <c r="C15" t="n">
-        <v>8725.929717772693</v>
+        <v>8898.606315789473</v>
       </c>
       <c r="D15" t="n">
-        <v>12009.27581998474</v>
+        <v>18683.4106101537</v>
+      </c>
+      <c r="E15" t="n">
+        <v>14658.52965222945</v>
+      </c>
+      <c r="F15" t="n">
+        <v>8105.464250277116</v>
+      </c>
+      <c r="G15" t="n">
+        <v>18892.19356662378</v>
+      </c>
+      <c r="H15" t="n">
+        <v>14652.03802416556</v>
+      </c>
+      <c r="I15" t="n">
+        <v>9028.16345977711</v>
+      </c>
+      <c r="J15" t="n">
+        <v>18976.15428733044</v>
+      </c>
+      <c r="K15" t="n">
+        <v>14658.63213477616</v>
+      </c>
+      <c r="L15" t="n">
+        <v>8105.782680750226</v>
+      </c>
+      <c r="M15" t="n">
+        <v>18892.49825989774</v>
+      </c>
+      <c r="N15" t="n">
+        <v>14568.75026552103</v>
+      </c>
+      <c r="O15" t="n">
+        <v>8974.793636396034</v>
+      </c>
+      <c r="P15" t="n">
+        <v>18882.42428191569</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>14658.6173803055</v>
+      </c>
+      <c r="R15" t="n">
+        <v>8105.6184385665</v>
+      </c>
+      <c r="S15" t="n">
+        <v>18892.27742016617</v>
+      </c>
+      <c r="T15" t="n">
+        <v>14652.0395959014</v>
+      </c>
+      <c r="U15" t="n">
+        <v>9028.16637737179</v>
+      </c>
+      <c r="V15" t="n">
+        <v>18976.1560007821</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_11_06_new.xlsx</t>
+          <t>HuGaDB_v2_various_10_12.xlsx</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>13969.6899188876</v>
+        <v>14675.19276887872</v>
       </c>
       <c r="C16" t="n">
-        <v>8975.213982232523</v>
+        <v>8725.929717772693</v>
       </c>
       <c r="D16" t="n">
-        <v>18275.19065276168</v>
+        <v>12009.27581998474</v>
+      </c>
+      <c r="E16" t="n">
+        <v>14699.92475516743</v>
+      </c>
+      <c r="F16" t="n">
+        <v>8905.982635604571</v>
+      </c>
+      <c r="G16" t="n">
+        <v>12304.0450043345</v>
+      </c>
+      <c r="H16" t="n">
+        <v>14652.43110696358</v>
+      </c>
+      <c r="I16" t="n">
+        <v>8810.959929997369</v>
+      </c>
+      <c r="J16" t="n">
+        <v>12010.87940824727</v>
+      </c>
+      <c r="K16" t="n">
+        <v>14699.99330189208</v>
+      </c>
+      <c r="L16" t="n">
+        <v>8906.282371675081</v>
+      </c>
+      <c r="M16" t="n">
+        <v>12304.42458442713</v>
+      </c>
+      <c r="N16" t="n">
+        <v>14665.06266911449</v>
+      </c>
+      <c r="O16" t="n">
+        <v>8942.547868864918</v>
+      </c>
+      <c r="P16" t="n">
+        <v>12150.21701142839</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>14699.95945407711</v>
+      </c>
+      <c r="R16" t="n">
+        <v>8906.085394571886</v>
+      </c>
+      <c r="S16" t="n">
+        <v>12304.08110519426</v>
+      </c>
+      <c r="T16" t="n">
+        <v>14652.43166870027</v>
+      </c>
+      <c r="U16" t="n">
+        <v>8810.961984578315</v>
+      </c>
+      <c r="V16" t="n">
+        <v>12010.88016080299</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_09_15_new.xlsx</t>
+          <t>HuGaDB_v2_various_10_11.xlsx</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>16991.83547683923</v>
+        <v>13521.21590909091</v>
       </c>
       <c r="C17" t="n">
-        <v>8402.440558583105</v>
+        <v>6497.654826203209</v>
       </c>
       <c r="D17" t="n">
-        <v>13867.38919618529</v>
+        <v>11926.52139037433</v>
+      </c>
+      <c r="E17" t="n">
+        <v>14184.94067066668</v>
+      </c>
+      <c r="F17" t="n">
+        <v>6230.425128075638</v>
+      </c>
+      <c r="G17" t="n">
+        <v>12284.91211975312</v>
+      </c>
+      <c r="H17" t="n">
+        <v>14181.9971366646</v>
+      </c>
+      <c r="I17" t="n">
+        <v>6734.517882142002</v>
+      </c>
+      <c r="J17" t="n">
+        <v>12247.97111287415</v>
+      </c>
+      <c r="K17" t="n">
+        <v>14185.0610450526</v>
+      </c>
+      <c r="L17" t="n">
+        <v>6230.778769503512</v>
+      </c>
+      <c r="M17" t="n">
+        <v>12285.24485257069</v>
+      </c>
+      <c r="N17" t="n">
+        <v>14222.85079702036</v>
+      </c>
+      <c r="O17" t="n">
+        <v>6610.238136271937</v>
+      </c>
+      <c r="P17" t="n">
+        <v>12246.81086236204</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>14185.00419056641</v>
+      </c>
+      <c r="R17" t="n">
+        <v>6230.561255801942</v>
+      </c>
+      <c r="S17" t="n">
+        <v>12284.94955070986</v>
+      </c>
+      <c r="T17" t="n">
+        <v>14181.99840714833</v>
+      </c>
+      <c r="U17" t="n">
+        <v>6734.520496453325</v>
+      </c>
+      <c r="V17" t="n">
+        <v>12247.97183587127</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_11_12_new.xlsx</t>
+          <t>HuGaDB_v2_various_10_09.xlsx</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>14351.42986384266</v>
+        <v>14805.45829984544</v>
       </c>
       <c r="C18" t="n">
-        <v>7413.231497730711</v>
+        <v>11356.70955177743</v>
       </c>
       <c r="D18" t="n">
-        <v>14693.29419062027</v>
+        <v>12075.04955177743</v>
+      </c>
+      <c r="E18" t="n">
+        <v>14895.80405659855</v>
+      </c>
+      <c r="F18" t="n">
+        <v>11491.3860954022</v>
+      </c>
+      <c r="G18" t="n">
+        <v>12448.90368397611</v>
+      </c>
+      <c r="H18" t="n">
+        <v>14787.72614365742</v>
+      </c>
+      <c r="I18" t="n">
+        <v>11470.58949442912</v>
+      </c>
+      <c r="J18" t="n">
+        <v>12033.95672566078</v>
+      </c>
+      <c r="K18" t="n">
+        <v>14895.91763110267</v>
+      </c>
+      <c r="L18" t="n">
+        <v>11491.6769412559</v>
+      </c>
+      <c r="M18" t="n">
+        <v>12449.31110266538</v>
+      </c>
+      <c r="N18" t="n">
+        <v>14829.99753140144</v>
+      </c>
+      <c r="O18" t="n">
+        <v>11662.33706789937</v>
+      </c>
+      <c r="P18" t="n">
+        <v>12200.09377248398</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>14895.85866828248</v>
+      </c>
+      <c r="R18" t="n">
+        <v>11491.4709091095</v>
+      </c>
+      <c r="S18" t="n">
+        <v>12448.94608480903</v>
+      </c>
+      <c r="T18" t="n">
+        <v>14787.72718748697</v>
+      </c>
+      <c r="U18" t="n">
+        <v>11470.59128932662</v>
+      </c>
+      <c r="V18" t="n">
+        <v>12033.9575772016</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_11_08_new.xlsx</t>
+          <t>HuGaDB_v2_various_09_16.xlsx</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>13297.47772048846</v>
+        <v>17312.43525076766</v>
       </c>
       <c r="C19" t="n">
-        <v>6853.419240162822</v>
+        <v>8609.975066530194</v>
       </c>
       <c r="D19" t="n">
-        <v>14886.5550339213</v>
+        <v>14215.28016376663</v>
+      </c>
+      <c r="E19" t="n">
+        <v>17778.6812072483</v>
+      </c>
+      <c r="F19" t="n">
+        <v>7665.049994232494</v>
+      </c>
+      <c r="G19" t="n">
+        <v>14493.01662326918</v>
+      </c>
+      <c r="H19" t="n">
+        <v>17760.51198740289</v>
+      </c>
+      <c r="I19" t="n">
+        <v>8752.920248064203</v>
+      </c>
+      <c r="J19" t="n">
+        <v>14456.86756899209</v>
+      </c>
+      <c r="K19" t="n">
+        <v>17778.74637238176</v>
+      </c>
+      <c r="L19" t="n">
+        <v>7665.465488965001</v>
+      </c>
+      <c r="M19" t="n">
+        <v>14493.43027245317</v>
+      </c>
+      <c r="N19" t="n">
+        <v>17742.28861950894</v>
+      </c>
+      <c r="O19" t="n">
+        <v>8507.370934637582</v>
+      </c>
+      <c r="P19" t="n">
+        <v>14430.07920777562</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>17778.77622685583</v>
+      </c>
+      <c r="R19" t="n">
+        <v>7665.210244987056</v>
+      </c>
+      <c r="S19" t="n">
+        <v>14493.11529198479</v>
+      </c>
+      <c r="T19" t="n">
+        <v>17760.51380734357</v>
+      </c>
+      <c r="U19" t="n">
+        <v>8752.923356958958</v>
+      </c>
+      <c r="V19" t="n">
+        <v>14456.86957998402</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_10_11_new.xlsx</t>
+          <t>HuGaDB_v2_various_11_08.xlsx</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>13521.21590909091</v>
+        <v>13297.47772048846</v>
       </c>
       <c r="C20" t="n">
-        <v>6497.654826203209</v>
+        <v>6853.419240162822</v>
       </c>
       <c r="D20" t="n">
-        <v>11926.52139037433</v>
+        <v>14886.5550339213</v>
+      </c>
+      <c r="E20" t="n">
+        <v>13360.04270468231</v>
+      </c>
+      <c r="F20" t="n">
+        <v>7099.227082758106</v>
+      </c>
+      <c r="G20" t="n">
+        <v>14812.53182376395</v>
+      </c>
+      <c r="H20" t="n">
+        <v>13325.75292282337</v>
+      </c>
+      <c r="I20" t="n">
+        <v>7007.992030873081</v>
+      </c>
+      <c r="J20" t="n">
+        <v>14804.00100501364</v>
+      </c>
+      <c r="K20" t="n">
+        <v>13360.08649117004</v>
+      </c>
+      <c r="L20" t="n">
+        <v>7099.51215634679</v>
+      </c>
+      <c r="M20" t="n">
+        <v>14812.76568172757</v>
+      </c>
+      <c r="N20" t="n">
+        <v>13329.69663270842</v>
+      </c>
+      <c r="O20" t="n">
+        <v>7218.801462888288</v>
+      </c>
+      <c r="P20" t="n">
+        <v>14782.67925628139</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>13360.07695939221</v>
+      </c>
+      <c r="R20" t="n">
+        <v>7099.349643848327</v>
+      </c>
+      <c r="S20" t="n">
+        <v>14812.6037909141</v>
+      </c>
+      <c r="T20" t="n">
+        <v>13325.7535798957</v>
+      </c>
+      <c r="U20" t="n">
+        <v>7007.994294610548</v>
+      </c>
+      <c r="V20" t="n">
+        <v>14804.00245670792</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_11_16_new.xlsx</t>
+          <t>HuGaDB_v2_various_10_10.xlsx</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>12847.03674698795</v>
+        <v>14622.96586490939</v>
       </c>
       <c r="C21" t="n">
-        <v>6106.498915662651</v>
+        <v>7959.212883031301</v>
       </c>
       <c r="D21" t="n">
-        <v>14903.65192771084</v>
+        <v>13524.69584843493</v>
+      </c>
+      <c r="E21" t="n">
+        <v>15389.46402112982</v>
+      </c>
+      <c r="F21" t="n">
+        <v>7295.255600859849</v>
+      </c>
+      <c r="G21" t="n">
+        <v>13920.17914273531</v>
+      </c>
+      <c r="H21" t="n">
+        <v>15440.14975510905</v>
+      </c>
+      <c r="I21" t="n">
+        <v>8205.694933241974</v>
+      </c>
+      <c r="J21" t="n">
+        <v>13874.92774354198</v>
+      </c>
+      <c r="K21" t="n">
+        <v>15389.64450305685</v>
+      </c>
+      <c r="L21" t="n">
+        <v>7295.632530635989</v>
+      </c>
+      <c r="M21" t="n">
+        <v>13920.5508046773</v>
+      </c>
+      <c r="N21" t="n">
+        <v>15545.40051450302</v>
+      </c>
+      <c r="O21" t="n">
+        <v>8078.922565339057</v>
+      </c>
+      <c r="P21" t="n">
+        <v>13857.49878890284</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>15389.53960156846</v>
+      </c>
+      <c r="R21" t="n">
+        <v>7295.372332853681</v>
+      </c>
+      <c r="S21" t="n">
+        <v>13920.22289766444</v>
+      </c>
+      <c r="T21" t="n">
+        <v>15440.15124332074</v>
+      </c>
+      <c r="U21" t="n">
+        <v>8205.697087580022</v>
+      </c>
+      <c r="V21" t="n">
+        <v>13874.92883092801</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_11_15_new.xlsx</t>
+          <t>HuGaDB_v2_various_11_12.xlsx</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>10976.76487804878</v>
+        <v>14351.42986384266</v>
       </c>
       <c r="C22" t="n">
-        <v>8074.643808630393</v>
+        <v>7413.231497730711</v>
       </c>
       <c r="D22" t="n">
-        <v>15927.9730956848</v>
+        <v>14693.29419062027</v>
+      </c>
+      <c r="E22" t="n">
+        <v>14386.79164764728</v>
+      </c>
+      <c r="F22" t="n">
+        <v>7665.238921165821</v>
+      </c>
+      <c r="G22" t="n">
+        <v>14584.48392878974</v>
+      </c>
+      <c r="H22" t="n">
+        <v>14335.83609508089</v>
+      </c>
+      <c r="I22" t="n">
+        <v>7667.086033463042</v>
+      </c>
+      <c r="J22" t="n">
+        <v>14568.19488539762</v>
+      </c>
+      <c r="K22" t="n">
+        <v>14386.84171150063</v>
+      </c>
+      <c r="L22" t="n">
+        <v>7665.567676279984</v>
+      </c>
+      <c r="M22" t="n">
+        <v>14584.73597698755</v>
+      </c>
+      <c r="N22" t="n">
+        <v>14324.69455417461</v>
+      </c>
+      <c r="O22" t="n">
+        <v>7897.646963285524</v>
+      </c>
+      <c r="P22" t="n">
+        <v>14545.46416618727</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>14386.85198012845</v>
+      </c>
+      <c r="R22" t="n">
+        <v>7665.360189246822</v>
+      </c>
+      <c r="S22" t="n">
+        <v>14584.56058895151</v>
+      </c>
+      <c r="T22" t="n">
+        <v>14335.83716731187</v>
+      </c>
+      <c r="U22" t="n">
+        <v>7667.088330055766</v>
+      </c>
+      <c r="V22" t="n">
+        <v>14568.19644396112</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_11_09_new.xlsx</t>
+          <t>HuGaDB_v2_various_09_15.xlsx</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>12244.06223968566</v>
+        <v>16991.83547683923</v>
       </c>
       <c r="C23" t="n">
-        <v>10508.59968565815</v>
+        <v>8402.440558583105</v>
       </c>
       <c r="D23" t="n">
-        <v>17132.17516699411</v>
+        <v>13867.38919618529</v>
+      </c>
+      <c r="E23" t="n">
+        <v>17552.53705141893</v>
+      </c>
+      <c r="F23" t="n">
+        <v>7261.280289790436</v>
+      </c>
+      <c r="G23" t="n">
+        <v>14167.77560744096</v>
+      </c>
+      <c r="H23" t="n">
+        <v>17507.83004620655</v>
+      </c>
+      <c r="I23" t="n">
+        <v>8524.415408810804</v>
+      </c>
+      <c r="J23" t="n">
+        <v>14085.00397517236</v>
+      </c>
+      <c r="K23" t="n">
+        <v>17552.62141440949</v>
+      </c>
+      <c r="L23" t="n">
+        <v>7261.665482749518</v>
+      </c>
+      <c r="M23" t="n">
+        <v>14168.16303644051</v>
+      </c>
+      <c r="N23" t="n">
+        <v>17494.13637362505</v>
+      </c>
+      <c r="O23" t="n">
+        <v>8264.312300491474</v>
+      </c>
+      <c r="P23" t="n">
+        <v>14093.77084397411</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>17552.64486609237</v>
+      </c>
+      <c r="R23" t="n">
+        <v>7261.454145490905</v>
+      </c>
+      <c r="S23" t="n">
+        <v>14167.86441886985</v>
+      </c>
+      <c r="T23" t="n">
+        <v>17507.83217758016</v>
+      </c>
+      <c r="U23" t="n">
+        <v>8524.418799396943</v>
+      </c>
+      <c r="V23" t="n">
+        <v>14085.00595543094</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_11_04_new.xlsx</t>
+          <t>HuGaDB_v2_various_11_09.xlsx</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>14340.75947834187</v>
+        <v>12244.06223968566</v>
       </c>
       <c r="C24" t="n">
-        <v>8898.606315789473</v>
+        <v>10508.59968565815</v>
       </c>
       <c r="D24" t="n">
-        <v>18683.4106101537</v>
+        <v>17132.17516699411</v>
+      </c>
+      <c r="E24" t="n">
+        <v>12782.26109010702</v>
+      </c>
+      <c r="F24" t="n">
+        <v>9274.891813038359</v>
+      </c>
+      <c r="G24" t="n">
+        <v>17607.03623555998</v>
+      </c>
+      <c r="H24" t="n">
+        <v>12972.94309056309</v>
+      </c>
+      <c r="I24" t="n">
+        <v>10665.14208547873</v>
+      </c>
+      <c r="J24" t="n">
+        <v>17637.04799325088</v>
+      </c>
+      <c r="K24" t="n">
+        <v>12782.44819947587</v>
+      </c>
+      <c r="L24" t="n">
+        <v>9275.25154929292</v>
+      </c>
+      <c r="M24" t="n">
+        <v>17607.36692815573</v>
+      </c>
+      <c r="N24" t="n">
+        <v>13068.50447538949</v>
+      </c>
+      <c r="O24" t="n">
+        <v>10518.54131893241</v>
+      </c>
+      <c r="P24" t="n">
+        <v>17593.76689485475</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>12782.36513437996</v>
+      </c>
+      <c r="R24" t="n">
+        <v>9275.01547818594</v>
+      </c>
+      <c r="S24" t="n">
+        <v>17607.13812052701</v>
+      </c>
+      <c r="T24" t="n">
+        <v>12972.94491615893</v>
+      </c>
+      <c r="U24" t="n">
+        <v>10665.14430019365</v>
+      </c>
+      <c r="V24" t="n">
+        <v>17637.04997703705</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_11_14_new.xlsx</t>
+          <t>HuGaDB_v2_various_11_07.xlsx</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>13772.42130718954</v>
+        <v>14126.36040194884</v>
       </c>
       <c r="C25" t="n">
-        <v>7509.6677124183</v>
+        <v>8918.031035322778</v>
       </c>
       <c r="D25" t="n">
-        <v>15607.93477124183</v>
+        <v>18398.5653593179</v>
+      </c>
+      <c r="E25" t="n">
+        <v>14516.8019642577</v>
+      </c>
+      <c r="F25" t="n">
+        <v>8191.432208487378</v>
+      </c>
+      <c r="G25" t="n">
+        <v>18579.85593416091</v>
+      </c>
+      <c r="H25" t="n">
+        <v>14488.87799929638</v>
+      </c>
+      <c r="I25" t="n">
+        <v>9067.426384341527</v>
+      </c>
+      <c r="J25" t="n">
+        <v>18686.45935206191</v>
+      </c>
+      <c r="K25" t="n">
+        <v>14516.90715780365</v>
+      </c>
+      <c r="L25" t="n">
+        <v>8191.751762087912</v>
+      </c>
+      <c r="M25" t="n">
+        <v>18580.13886819503</v>
+      </c>
+      <c r="N25" t="n">
+        <v>14422.74987803857</v>
+      </c>
+      <c r="O25" t="n">
+        <v>9034.249558861406</v>
+      </c>
+      <c r="P25" t="n">
+        <v>18582.95992131368</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>14516.87601718912</v>
+      </c>
+      <c r="R25" t="n">
+        <v>8191.579370075506</v>
+      </c>
+      <c r="S25" t="n">
+        <v>18579.93733624318</v>
+      </c>
+      <c r="T25" t="n">
+        <v>14488.87929231702</v>
+      </c>
+      <c r="U25" t="n">
+        <v>9067.429271857065</v>
+      </c>
+      <c r="V25" t="n">
+        <v>18686.46101537714</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>HuGaDB_v2_various_09_13_new.xlsx</t>
+          <t>HuGaDB_v2_various_11_13.xlsx</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>17625.44300904977</v>
+        <v>11319.16363468635</v>
       </c>
       <c r="C26" t="n">
-        <v>8249.661063348416</v>
+        <v>9104.747859778598</v>
       </c>
       <c r="D26" t="n">
-        <v>14519.2603959276</v>
+        <v>17086.89215867158</v>
+      </c>
+      <c r="E26" t="n">
+        <v>11925.7657592112</v>
+      </c>
+      <c r="F26" t="n">
+        <v>7906.498119374387</v>
+      </c>
+      <c r="G26" t="n">
+        <v>17566.53361833888</v>
+      </c>
+      <c r="H26" t="n">
+        <v>11948.18578511895</v>
+      </c>
+      <c r="I26" t="n">
+        <v>9261.689578317937</v>
+      </c>
+      <c r="J26" t="n">
+        <v>17624.31832554604</v>
+      </c>
+      <c r="K26" t="n">
+        <v>11925.91993399213</v>
+      </c>
+      <c r="L26" t="n">
+        <v>7906.794438010802</v>
+      </c>
+      <c r="M26" t="n">
+        <v>17566.79023561753</v>
+      </c>
+      <c r="N26" t="n">
+        <v>11924.43212721144</v>
+      </c>
+      <c r="O26" t="n">
+        <v>9029.910939334359</v>
+      </c>
+      <c r="P26" t="n">
+        <v>17569.75755116513</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>11925.83780546995</v>
+      </c>
+      <c r="R26" t="n">
+        <v>7906.618344999494</v>
+      </c>
+      <c r="S26" t="n">
+        <v>17566.59872209765</v>
+      </c>
+      <c r="T26" t="n">
+        <v>11948.18723882691</v>
+      </c>
+      <c r="U26" t="n">
+        <v>9261.691857275333</v>
+      </c>
+      <c r="V26" t="n">
+        <v>17624.31970955924</v>
       </c>
     </row>
   </sheetData>

</xml_diff>